<commit_message>
updated TSS sites based on the discrepany between v3 and v4 of the Putida genome
</commit_message>
<xml_diff>
--- a/primary TSS.xlsx
+++ b/primary TSS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukez\Desktop\Winter 2020 Rotation\TSS analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66778ABD-B5B7-48C2-BBC6-840BBAD582E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F7FBD1-74FA-4FC9-896D-80BFA85E9058}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="1305" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -6435,8 +6435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1307CF93-B963-4D5C-8DB7-8C5894DD131A}">
   <dimension ref="B1:L4569"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A941" workbookViewId="0">
+      <selection activeCell="F953" sqref="F953"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>